<commit_message>
Pushing the new changes done in Sports Module
</commit_message>
<xml_diff>
--- a/Automation-Framework-BookMyShow/ExecutionFiles/Run/BookMyShow.xlsx
+++ b/Automation-Framework-BookMyShow/ExecutionFiles/Run/BookMyShow.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="214">
   <si>
     <t>ProjectName</t>
   </si>
@@ -1007,12 +1007,14 @@
   <si>
     <t>Japanese</t>
   </si>
+  <si>
+    <t>Price</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1553,10 +1555,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.33203125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="24.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="37.44140625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="83.6640625" collapsed="false"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" customWidth="1"/>
+    <col min="4" max="4" width="83.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1658,20 +1660,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="9" width="12.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="9" width="12.88671875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="9" width="14.33203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="17" width="49.5546875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="10" width="49.5546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="34" width="49.5546875" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="9" width="45.88671875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="34" width="44.33203125" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="34" width="42.109375" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="17" width="19.88671875" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" style="9" width="24.109375" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="14.88671875" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="18.88671875" collapsed="false"/>
+    <col min="1" max="1" width="12.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="49.5546875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="49.5546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="49.5546875" style="34" customWidth="1"/>
+    <col min="8" max="8" width="45.88671875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="44.33203125" style="34" customWidth="1"/>
+    <col min="10" max="10" width="42.109375" style="34" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" style="17" customWidth="1"/>
+    <col min="12" max="12" width="24.109375" style="9" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -2635,11 +2637,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="13.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="9" width="19.6640625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="48.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="18.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="20.5546875" collapsed="false"/>
+    <col min="1" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2762,11 +2764,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="9" width="50.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="9" width="21.88671875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="9" width="17.5546875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="10" width="47.44140625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="34" width="77.109375" collapsed="false"/>
+    <col min="1" max="1" width="50" style="9" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="47.44140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="77.109375" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -2920,12 +2922,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="9" width="10.109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="15.5546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="10" width="76.6640625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="31.6640625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="9" width="40.109375" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="29.44140625" collapsed="false"/>
+    <col min="1" max="1" width="10.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="76.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3061,24 +3063,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.88671875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="40.0" collapsed="false"/>
+    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>201</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>202</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
@@ -3086,42 +3092,42 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>212</v>
       </c>

</xml_diff>

<commit_message>
commenting the utility classes
</commit_message>
<xml_diff>
--- a/Automation-Framework-BookMyShow/ExecutionFiles/Run/BookMyShow.xlsx
+++ b/Automation-Framework-BookMyShow/ExecutionFiles/Run/BookMyShow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16416" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16416" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalVariables" sheetId="2" r:id="rId1"/>
@@ -1579,10 +1579,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="37.44140625" customWidth="1"/>
-    <col min="4" max="4" width="83.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="83.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1678,26 +1678,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="49.5546875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="49.5546875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="49.5546875" style="34" customWidth="1"/>
-    <col min="8" max="8" width="45.88671875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="44.33203125" style="34" customWidth="1"/>
-    <col min="10" max="10" width="42.109375" style="34" customWidth="1"/>
-    <col min="11" max="11" width="19.88671875" style="17" customWidth="1"/>
-    <col min="12" max="12" width="24.109375" style="9" customWidth="1"/>
-    <col min="13" max="13" width="14.88671875" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.88671875" style="9" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.33203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.5546875" style="10" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="49.5546875" style="34" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.88671875" style="9" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="44.33203125" style="34" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="42.109375" style="34" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.88671875" style="17" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.109375" style="9" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -2578,17 +2578,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="1" max="2" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="48" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2731,11 +2731,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50" style="9" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="47.44140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="77.109375" style="34" customWidth="1"/>
+    <col min="1" max="1" width="50" style="9" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.88671875" style="9" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.5546875" style="9" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.44140625" style="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="77.109375" style="34" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -2889,12 +2889,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="76.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="5" width="40.109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="9" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="76.6640625" style="10" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="40.109375" style="9" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3030,17 +3030,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -3114,17 +3114,17 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
@@ -3134,7 +3134,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
@@ -3144,7 +3144,7 @@
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>